<commit_message>
"intervalo fecha analizador lexico"
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/TABLATOKENS.xlsx
+++ b/DOCUMENTACION/TABLATOKENS.xlsx
@@ -128,9 +128,6 @@
     <t xml:space="preserve">nombre equipo </t>
   </si>
   <si>
-    <t>nombre archivo</t>
-  </si>
-  <si>
     <t xml:space="preserve">numero </t>
   </si>
   <si>
@@ -218,9 +215,6 @@
     <t>TOP</t>
   </si>
   <si>
-    <t>pr_resultado equipo pr_vs equipo pr_temporada fecha</t>
-  </si>
-  <si>
     <t xml:space="preserve">pr_jornada numero pr_temporada fecha </t>
   </si>
   <si>
@@ -264,6 +258,12 @@
   </si>
   <si>
     <t>pr_partidos equipo pr_temporada fecha pr_flagF archivo pr_flagApartir numero pr_flagHasta numero</t>
+  </si>
+  <si>
+    <t>identificador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pr_resultado equipo pr_vs equipo pr_temporada fecha </t>
   </si>
 </sst>
 </file>
@@ -366,11 +366,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -654,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,24 +670,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="G1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="G1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="4" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
@@ -703,17 +703,17 @@
         <v>3</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="5" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -726,10 +726,10 @@
         <v>4</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>4</v>
@@ -743,21 +743,21 @@
         <v>33</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -771,14 +771,14 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -792,7 +792,7 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>18</v>
@@ -806,38 +806,38 @@
         <v>32</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
@@ -845,16 +845,16 @@
         <v>7</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" s="7">
         <v>20</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>25</v>
@@ -865,7 +865,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>12</v>
@@ -879,26 +879,26 @@
         <v>13</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="D13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -912,11 +912,11 @@
       </c>
     </row>
     <row r="15" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>15</v>
@@ -928,18 +928,18 @@
         <v>11</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>16</v>
@@ -948,18 +948,18 @@
         <v>16</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>17</v>
@@ -969,11 +969,11 @@
       </c>
     </row>
     <row r="18" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>18</v>
@@ -985,14 +985,14 @@
         <v>14</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -1005,10 +1005,10 @@
         <v>19</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
@@ -1016,7 +1016,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>20</v>
@@ -1025,10 +1025,10 @@
         <v>20</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1036,7 +1036,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>21</v>
@@ -1046,11 +1046,11 @@
       </c>
     </row>
     <row r="22" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>22</v>
@@ -1062,30 +1062,30 @@
         <v>18</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>23</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1093,7 +1093,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>24</v>
@@ -1103,11 +1103,11 @@
       </c>
     </row>
     <row r="25" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>25</v>
@@ -1124,61 +1124,61 @@
         <v>19</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="H27" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="H28" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="G30" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="H31" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="H32" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="H33" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
@@ -1186,10 +1186,10 @@
         <v>25</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>